<commit_message>
fix analysis unit table
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/11_EntityType.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/11_EntityType.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="97245" yWindow="0" windowWidth="20490" windowHeight="7155" tabRatio="949" activeTab="10"/>
+    <workbookView xWindow="97245" yWindow="0" windowWidth="20490" windowHeight="7155" tabRatio="949" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -679,9 +679,6 @@
     <t>Hourly</t>
   </si>
   <si>
-    <t>Properties_Predictive</t>
-  </si>
-  <si>
     <t>LastUpdateAnalysisUnit</t>
   </si>
   <si>
@@ -824,6 +821,9 @@
   </si>
   <si>
     <t>Only for String, Boolean, Real, Integer, Date with Value pattern = Range</t>
+  </si>
+  <si>
+    <t>Analysis_Unit</t>
   </si>
 </sst>
 </file>
@@ -1289,7 +1289,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1299,12 +1299,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFAC2524"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1320,7 +1314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1493,7 +1487,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2342,8 +2335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -2368,59 +2361,59 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="67" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="67" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" s="67" t="s">
-        <v>66</v>
+      <c r="C2" s="66" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="66" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="66" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="67" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" s="67" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" s="67" t="s">
-        <v>71</v>
+      <c r="A3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="66" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="66" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="66" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="66" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" s="67" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" s="67" t="s">
-        <v>74</v>
-      </c>
-      <c r="D4" s="67" t="s">
-        <v>74</v>
+      <c r="A4" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="66" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="66" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="66" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2434,8 +2427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D32"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -2465,7 +2458,7 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -2475,7 +2468,7 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -2485,7 +2478,7 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -2495,7 +2488,7 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -2505,7 +2498,7 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
@@ -2515,13 +2508,13 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C7" t="s">
         <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2529,13 +2522,13 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C8" t="s">
         <v>59</v>
       </c>
       <c r="D8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2543,13 +2536,13 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C9" t="s">
         <v>59</v>
       </c>
       <c r="D9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2557,13 +2550,13 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C10" t="s">
         <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2571,13 +2564,13 @@
         <v>24</v>
       </c>
       <c r="B11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" t="s">
         <v>86</v>
-      </c>
-      <c r="C11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2585,7 +2578,7 @@
         <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C12"/>
       <c r="D12"/>
@@ -2595,13 +2588,13 @@
         <v>26</v>
       </c>
       <c r="B13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" t="s">
         <v>89</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>90</v>
-      </c>
-      <c r="D13" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2609,13 +2602,13 @@
         <v>27</v>
       </c>
       <c r="B14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" t="s">
         <v>92</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>93</v>
-      </c>
-      <c r="D14" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2623,13 +2616,13 @@
         <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C15" t="s">
         <v>59</v>
       </c>
       <c r="D15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2637,13 +2630,13 @@
         <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C16" t="s">
         <v>59</v>
       </c>
       <c r="D16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2651,7 +2644,7 @@
         <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C17"/>
       <c r="D17"/>
@@ -2661,7 +2654,7 @@
         <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C18"/>
       <c r="D18"/>
@@ -2671,13 +2664,13 @@
         <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C19" t="s">
         <v>59</v>
       </c>
       <c r="D19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2685,13 +2678,13 @@
         <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C20" t="s">
         <v>59</v>
       </c>
       <c r="D20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2699,13 +2692,13 @@
         <v>34</v>
       </c>
       <c r="B21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" t="s">
         <v>98</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>99</v>
-      </c>
-      <c r="D21" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2713,13 +2706,13 @@
         <v>35</v>
       </c>
       <c r="B22" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" t="s">
         <v>101</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>102</v>
-      </c>
-      <c r="D22" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2727,7 +2720,7 @@
         <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C23"/>
       <c r="D23"/>
@@ -2737,13 +2730,13 @@
         <v>37</v>
       </c>
       <c r="B24" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" t="s">
         <v>105</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>106</v>
-      </c>
-      <c r="D24" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2751,10 +2744,10 @@
         <v>38</v>
       </c>
       <c r="B25" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" t="s">
         <v>108</v>
-      </c>
-      <c r="C25" t="s">
-        <v>109</v>
       </c>
       <c r="D25"/>
     </row>
@@ -2763,13 +2756,13 @@
         <v>39</v>
       </c>
       <c r="B26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C26" t="s">
         <v>60</v>
       </c>
       <c r="D26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2777,7 +2770,7 @@
         <v>40</v>
       </c>
       <c r="B27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
@@ -2787,13 +2780,13 @@
         <v>41</v>
       </c>
       <c r="B28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C28" t="s">
         <v>59</v>
       </c>
       <c r="D28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2801,7 +2794,7 @@
         <v>42</v>
       </c>
       <c r="B29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C29"/>
       <c r="D29"/>
@@ -2811,7 +2804,7 @@
         <v>43</v>
       </c>
       <c r="B30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C30"/>
       <c r="D30"/>
@@ -2821,7 +2814,7 @@
         <v>44</v>
       </c>
       <c r="B31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C31"/>
       <c r="D31"/>
@@ -2831,13 +2824,13 @@
         <v>45</v>
       </c>
       <c r="B32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C32" t="s">
         <v>58</v>
       </c>
       <c r="D32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2952,8 +2945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE5"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -3057,19 +3050,19 @@
       </c>
     </row>
     <row r="2" spans="1:31" s="65" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="67" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="67" t="s">
+      <c r="C2" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="67" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2" s="68">
+      <c r="D2" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="67">
         <v>4</v>
       </c>
       <c r="F2" s="65" t="s">
@@ -3085,16 +3078,16 @@
         <v>58</v>
       </c>
       <c r="J2" s="65" t="s">
-        <v>70</v>
-      </c>
-      <c r="L2" s="69"/>
-      <c r="N2" s="69"/>
+        <v>69</v>
+      </c>
+      <c r="L2" s="68"/>
+      <c r="N2" s="68"/>
       <c r="O2" s="65" t="s">
         <v>58</v>
       </c>
-      <c r="P2" s="69"/>
+      <c r="P2" s="68"/>
       <c r="Q2" s="65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="R2" s="65" t="s">
         <v>59</v>
@@ -3105,35 +3098,35 @@
       <c r="T2" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="U2" s="69"/>
-      <c r="V2" s="69"/>
-      <c r="W2" s="69"/>
-      <c r="X2" s="69"/>
+      <c r="U2" s="68"/>
+      <c r="V2" s="68"/>
+      <c r="W2" s="68"/>
+      <c r="X2" s="68"/>
       <c r="Y2" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="Z2" s="69"/>
-      <c r="AA2" s="69"/>
-      <c r="AC2" s="69"/>
-      <c r="AD2" s="69"/>
+      <c r="Z2" s="68"/>
+      <c r="AA2" s="68"/>
+      <c r="AC2" s="68"/>
+      <c r="AD2" s="68"/>
       <c r="AE2" s="65" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A3" s="67" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="67" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" s="67" t="s">
+      <c r="A3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="66" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="67" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" s="68">
+      <c r="D3" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="67">
         <v>5</v>
       </c>
       <c r="F3" s="65" t="s">
@@ -3149,18 +3142,18 @@
         <v>58</v>
       </c>
       <c r="J3" s="65" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K3" s="65"/>
-      <c r="L3" s="69"/>
+      <c r="L3" s="68"/>
       <c r="M3" s="65"/>
-      <c r="N3" s="69"/>
+      <c r="N3" s="68"/>
       <c r="O3" s="65" t="s">
         <v>58</v>
       </c>
-      <c r="P3" s="69"/>
+      <c r="P3" s="68"/>
       <c r="Q3" s="65" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R3" s="65" t="s">
         <v>59</v>
@@ -3171,36 +3164,36 @@
       <c r="T3" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="U3" s="69"/>
-      <c r="V3" s="69"/>
-      <c r="W3" s="69"/>
-      <c r="X3" s="69"/>
+      <c r="U3" s="68"/>
+      <c r="V3" s="68"/>
+      <c r="W3" s="68"/>
+      <c r="X3" s="68"/>
       <c r="Y3" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="Z3" s="69"/>
-      <c r="AA3" s="69"/>
+      <c r="Z3" s="68"/>
+      <c r="AA3" s="68"/>
       <c r="AB3" s="65"/>
-      <c r="AC3" s="69"/>
-      <c r="AD3" s="69"/>
+      <c r="AC3" s="68"/>
+      <c r="AD3" s="68"/>
       <c r="AE3" s="65" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A4" s="67" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" s="67" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" s="67" t="s">
+      <c r="A4" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="66" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="67" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" s="68">
+      <c r="D4" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="67">
         <v>6</v>
       </c>
       <c r="F4" s="65" t="s">
@@ -3216,18 +3209,18 @@
         <v>58</v>
       </c>
       <c r="J4" s="65" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K4" s="65"/>
-      <c r="L4" s="69"/>
+      <c r="L4" s="68"/>
       <c r="M4" s="65"/>
-      <c r="N4" s="69"/>
+      <c r="N4" s="68"/>
       <c r="O4" s="65" t="s">
         <v>58</v>
       </c>
-      <c r="P4" s="69"/>
+      <c r="P4" s="68"/>
       <c r="Q4" s="65" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="R4" s="65" t="s">
         <v>59</v>
@@ -3238,34 +3231,34 @@
       <c r="T4" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="U4" s="69"/>
-      <c r="V4" s="69"/>
-      <c r="W4" s="69"/>
-      <c r="X4" s="69"/>
+      <c r="U4" s="68"/>
+      <c r="V4" s="68"/>
+      <c r="W4" s="68"/>
+      <c r="X4" s="68"/>
       <c r="Y4" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="Z4" s="69"/>
-      <c r="AA4" s="69"/>
+      <c r="Z4" s="68"/>
+      <c r="AA4" s="68"/>
       <c r="AB4" s="65"/>
-      <c r="AC4" s="69"/>
-      <c r="AD4" s="69"/>
+      <c r="AC4" s="68"/>
+      <c r="AD4" s="68"/>
       <c r="AE4" s="65" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="E5" s="1">
         <v>3</v>
@@ -3350,27 +3343,27 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="65" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="65" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>